<commit_message>
added necessary UI-Frames and update Projekplan/To-DO
</commit_message>
<xml_diff>
--- a/Meilensteine_Projektplan/Projektplan und Agenda.xlsx
+++ b/Meilensteine_Projektplan/Projektplan und Agenda.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10409"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10514"/>
   <workbookPr codeName="ThisWorkbook" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/alba/Desktop/Uni/6. Semester/Mobile Computing /MoCo_SoSe23_Projekt/Krasniqi_Osaj_AmirKhanian_MoCo_SoSe23-1/Meilensteine_Projektplan/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/alba/Desktop/Uni/6. Semester/Mobile Computing /Krasniqi_Osaj_AmirKhanian_MoCo_SoSe23/Meilensteine_Projektplan/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{E0970DA6-35AE-CC40-AF28-A6AFC776F6D9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{17B65F1A-A93B-D343-A3E2-8E6F81FFF8D2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="4020" yWindow="500" windowWidth="28800" windowHeight="22300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -18,7 +18,7 @@
   <definedNames>
     <definedName name="_xlnm.Print_Titles" localSheetId="0">AUFGABEN!$2:$2</definedName>
   </definedNames>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -26,7 +26,12 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
       </xcalcf:calcFeatures>
     </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
@@ -37,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="18">
   <si>
     <t>Vorgang</t>
   </si>
@@ -80,6 +85,18 @@
   <si>
     <t>Projekidee in Read.me Beschrieben</t>
   </si>
+  <si>
+    <t>UI-Frames Feinschliff</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Code UI Frame "HelloName" </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Updat:  NewPlant, New: Plantfamily, Careplan</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Nötife UI Frames in Figma erstellt </t>
+  </si>
 </sst>
 </file>
 
@@ -92,7 +109,7 @@
     <numFmt numFmtId="165" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="166" formatCode="&quot;Fertig&quot;;&quot;&quot;;&quot;&quot;"/>
   </numFmts>
-  <fonts count="20" x14ac:knownFonts="1">
+  <fonts count="21" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -240,6 +257,12 @@
       <color theme="5" tint="-0.249977111117893"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -639,32 +662,44 @@
     <xf numFmtId="0" fontId="4" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="6" applyFont="1" applyBorder="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="4" fillId="0" borderId="10" xfId="5" applyBorder="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="10" xfId="4" applyFont="1" applyBorder="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="10" xfId="3" applyFont="1" applyBorder="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="10" xfId="6" applyBorder="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="35" borderId="10" xfId="2" applyNumberFormat="1" applyFill="1" applyBorder="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="35" borderId="10" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="18" fillId="34" borderId="10" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="6" applyFont="1" applyBorder="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="6" applyFill="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="14" fontId="4" fillId="0" borderId="10" xfId="5" applyBorder="1">
+    <xf numFmtId="14" fontId="4" fillId="0" borderId="0" xfId="5" applyFill="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="10" xfId="4" applyFont="1" applyBorder="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="10" xfId="3" applyFont="1" applyBorder="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="10" xfId="6" applyBorder="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="35" borderId="10" xfId="2" applyNumberFormat="1" applyFill="1" applyBorder="1">
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="35" borderId="10" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1">
+    <xf numFmtId="166" fontId="20" fillId="0" borderId="0" xfId="3" applyFont="1" applyFill="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -722,13 +757,6 @@
   </cellStyles>
   <dxfs count="18">
     <dxf>
-      <border outline="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-      </border>
-    </dxf>
-    <dxf>
       <font>
         <b val="0"/>
         <i val="0"/>
@@ -744,11 +772,6 @@
         <name val="Calibri"/>
         <scheme val="minor"/>
       </font>
-      <border outline="0">
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-      </border>
     </dxf>
     <dxf>
       <font>
@@ -768,88 +791,6 @@
       </font>
     </dxf>
     <dxf>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right/>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical style="thin">
-          <color indexed="64"/>
-        </vertical>
-        <horizontal style="thin">
-          <color indexed="64"/>
-        </horizontal>
-      </border>
-    </dxf>
-    <dxf>
       <numFmt numFmtId="0" formatCode="General"/>
       <fill>
         <patternFill patternType="solid">
@@ -859,31 +800,10 @@
       </fill>
     </dxf>
     <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="8" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="8" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
+      <border outline="0">
         <left style="thin">
           <color indexed="64"/>
         </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top/>
-        <bottom/>
       </border>
     </dxf>
     <dxf>
@@ -919,6 +839,102 @@
         <name val="Calibri"/>
         <scheme val="minor"/>
       </font>
+      <border outline="0">
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+      </border>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="8" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right/>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
     </dxf>
     <dxf>
       <border diagonalUp="0" diagonalDown="0">
@@ -982,6 +998,25 @@
         <horizontal style="thin">
           <color indexed="64"/>
         </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="8" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top/>
+        <bottom/>
       </border>
     </dxf>
     <dxf>
@@ -1065,13 +1100,13 @@
     <xdr:from>
       <xdr:col>1</xdr:col>
       <xdr:colOff>38100</xdr:colOff>
-      <xdr:row>17</xdr:row>
+      <xdr:row>20</xdr:row>
       <xdr:rowOff>190499</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>8</xdr:col>
       <xdr:colOff>139700</xdr:colOff>
-      <xdr:row>37</xdr:row>
+      <xdr:row>40</xdr:row>
       <xdr:rowOff>140138</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -1109,17 +1144,17 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Aufgaben" displayName="Aufgaben" ref="B2:G5" totalsRowShown="0" headerRowDxfId="8">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Aufgaben" displayName="Aufgaben" ref="B2:G5" totalsRowShown="0" headerRowDxfId="13">
   <autoFilter ref="B2:G5" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
   <tableColumns count="6">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Nora Krasniqi" dataDxfId="13" dataCellStyle="Tabellentext"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="ANFANGSDATUM" dataDxfId="12" dataCellStyle="Datum"/>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="FÄLLIGKEITSDATUM" dataDxfId="11" dataCellStyle="Datum"/>
-    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="% ABGESCHLOSSEN" dataDxfId="4"/>
-    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0000-000007000000}" name="FERTIG" dataDxfId="5" dataCellStyle="Fertig">
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Nora Krasniqi" dataDxfId="12" dataCellStyle="Tabellentext"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="ANFANGSDATUM" dataDxfId="11" dataCellStyle="Datum"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="FÄLLIGKEITSDATUM" dataDxfId="10" dataCellStyle="Datum"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="% ABGESCHLOSSEN" dataDxfId="9"/>
+    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0000-000007000000}" name="FERTIG" dataDxfId="8" dataCellStyle="Fertig">
       <calculatedColumnFormula>--(Aufgaben[[#This Row],[% ABGESCHLOSSEN]]&gt;=1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0000-000008000000}" name="NOTIZEN" dataDxfId="3" dataCellStyle="Tabellentext"/>
+    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0000-000008000000}" name="NOTIZEN" dataDxfId="7" dataCellStyle="Tabellentext"/>
   </tableColumns>
   <tableStyleInfo name="Aufgabenliste" showFirstColumn="1" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
   <extLst>
@@ -1131,17 +1166,17 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{9F47294E-D73F-9E40-842D-FA65D389DB70}" name="Aufgaben4" displayName="Aufgaben4" ref="B6:G9" totalsRowShown="0" headerRowDxfId="7">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{9F47294E-D73F-9E40-842D-FA65D389DB70}" name="Aufgaben4" displayName="Aufgaben4" ref="B6:G9" totalsRowShown="0" headerRowDxfId="6">
   <autoFilter ref="B6:G9" xr:uid="{9F47294E-D73F-9E40-842D-FA65D389DB70}"/>
   <tableColumns count="6">
     <tableColumn id="1" xr3:uid="{9F89A8E0-9D9F-F44D-8776-0DAAD5AF9EBF}" name="Losik Amir Khanian" dataCellStyle="Tabellentext"/>
     <tableColumn id="4" xr3:uid="{D213AABD-C212-E049-A161-8ED70DDF41E6}" name="ANFANGSDATUM" dataCellStyle="Datum"/>
     <tableColumn id="5" xr3:uid="{6BC6B0FC-4052-3C4A-966E-F63BECA2512F}" name="FÄLLIGKEITSDATUM" dataCellStyle="Datum"/>
-    <tableColumn id="6" xr3:uid="{9D27484A-C280-2340-8907-07C37E7D9606}" name="% ABGESCHLOSSEN" dataDxfId="1"/>
-    <tableColumn id="7" xr3:uid="{6A8520DC-BE29-7540-BD65-6CB47AC68A02}" name="FERTIG" dataDxfId="2" dataCellStyle="Fertig">
+    <tableColumn id="6" xr3:uid="{9D27484A-C280-2340-8907-07C37E7D9606}" name="% ABGESCHLOSSEN" dataDxfId="5"/>
+    <tableColumn id="7" xr3:uid="{6A8520DC-BE29-7540-BD65-6CB47AC68A02}" name="FERTIG" dataDxfId="4" dataCellStyle="Fertig">
       <calculatedColumnFormula>--(Aufgaben4[[#This Row],[% ABGESCHLOSSEN]]&gt;=1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="8" xr3:uid="{56C8B5E3-E95C-7941-BD9B-1369BB3409EF}" name="NOTIZEN" dataDxfId="0" dataCellStyle="Tabellentext"/>
+    <tableColumn id="8" xr3:uid="{56C8B5E3-E95C-7941-BD9B-1369BB3409EF}" name="NOTIZEN" dataDxfId="3" dataCellStyle="Tabellentext"/>
   </tableColumns>
   <tableStyleInfo name="Aufgabenliste" showFirstColumn="1" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
   <extLst>
@@ -1153,14 +1188,14 @@
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{AFF70C9B-DCEA-ED4B-B164-EAE9BA931217}" name="Aufgaben5" displayName="Aufgaben5" ref="B10:G13" totalsRowShown="0" headerRowDxfId="6">
-  <autoFilter ref="B10:G13" xr:uid="{AFF70C9B-DCEA-ED4B-B164-EAE9BA931217}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{AFF70C9B-DCEA-ED4B-B164-EAE9BA931217}" name="Aufgaben5" displayName="Aufgaben5" ref="B10:G16" totalsRowShown="0" headerRowDxfId="2">
+  <autoFilter ref="B10:G16" xr:uid="{AFF70C9B-DCEA-ED4B-B164-EAE9BA931217}"/>
   <tableColumns count="6">
     <tableColumn id="1" xr3:uid="{E4CA5E25-C248-5C44-9D4F-58EE6BE537AE}" name="Alberije Osaj " dataCellStyle="Tabellentext"/>
     <tableColumn id="4" xr3:uid="{D2AFBDAD-C91B-9540-ABA2-967CEE81D618}" name="ANFANGSDATUM" dataCellStyle="Datum"/>
     <tableColumn id="5" xr3:uid="{E6FC5392-646E-554B-9E2B-CF376B866317}" name="FÄLLIGKEITSDATUM" dataCellStyle="Datum"/>
-    <tableColumn id="6" xr3:uid="{5FC0A8B2-9FC1-E745-9A72-488D0044612A}" name="% ABGESCHLOSSEN" dataDxfId="10"/>
-    <tableColumn id="7" xr3:uid="{BB41D1D3-823F-F54F-A416-6AC7AE779AC0}" name="FERTIG" dataDxfId="9" dataCellStyle="Fertig">
+    <tableColumn id="6" xr3:uid="{5FC0A8B2-9FC1-E745-9A72-488D0044612A}" name="% ABGESCHLOSSEN" dataDxfId="1"/>
+    <tableColumn id="7" xr3:uid="{BB41D1D3-823F-F54F-A416-6AC7AE779AC0}" name="FERTIG" dataDxfId="0" dataCellStyle="Fertig">
       <calculatedColumnFormula>--(Aufgaben5[[#This Row],[% ABGESCHLOSSEN]]&gt;=1)</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="8" xr3:uid="{92B6B262-0F93-AB48-A296-6217493C949E}" name="NOTIZEN" dataCellStyle="Tabellentext"/>
@@ -1381,10 +1416,10 @@
     <tabColor theme="4"/>
     <pageSetUpPr autoPageBreaks="0" fitToPage="1"/>
   </sheetPr>
-  <dimension ref="B1:G13"/>
+  <dimension ref="B1:G16"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="L7" sqref="L7"/>
+      <selection activeCell="J17" sqref="J17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.5" defaultRowHeight="33" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1400,252 +1435,300 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="C1" s="1"/>
-      <c r="D1" s="1"/>
-      <c r="E1" s="1"/>
-      <c r="F1" s="1"/>
-      <c r="G1" s="1"/>
+      <c r="C1" s="8"/>
+      <c r="D1" s="8"/>
+      <c r="E1" s="8"/>
+      <c r="F1" s="8"/>
+      <c r="G1" s="8"/>
     </row>
     <row r="2" spans="2:7" ht="25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B2" s="7" t="s">
+      <c r="B2" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="C2" s="7" t="s">
+      <c r="C2" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="D2" s="7" t="s">
+      <c r="D2" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="E2" s="7" t="s">
+      <c r="E2" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="F2" s="8" t="s">
+      <c r="F2" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="G2" s="7" t="s">
+      <c r="G2" s="6" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="3" spans="2:7" ht="33" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B3" s="2" t="s">
+      <c r="B3" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C3" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="D3" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="E3" s="4">
+      <c r="C3" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="E3" s="3">
         <v>0</v>
       </c>
-      <c r="F3" s="5">
+      <c r="F3" s="4">
         <f>--(Aufgaben[[#This Row],[% ABGESCHLOSSEN]]&gt;=1)</f>
         <v>0</v>
       </c>
-      <c r="G3" s="6"/>
+      <c r="G3" s="5"/>
     </row>
     <row r="4" spans="2:7" ht="33" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B4" s="6" t="s">
+      <c r="B4" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="C4" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="D4" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="E4" s="4">
+      <c r="C4" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="E4" s="3">
         <v>0</v>
       </c>
-      <c r="F4" s="5">
+      <c r="F4" s="4">
         <f>--(Aufgaben[[#This Row],[% ABGESCHLOSSEN]]&gt;=1)</f>
         <v>0</v>
       </c>
-      <c r="G4" s="6"/>
+      <c r="G4" s="5"/>
     </row>
     <row r="5" spans="2:7" ht="33" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B5" s="6" t="s">
+      <c r="B5" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="C5" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="D5" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="E5" s="4">
+      <c r="C5" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="E5" s="3">
         <v>0</v>
       </c>
-      <c r="F5" s="5">
+      <c r="F5" s="4">
         <f>--(Aufgaben[[#This Row],[% ABGESCHLOSSEN]]&gt;=1)</f>
         <v>0</v>
       </c>
-      <c r="G5" s="6"/>
+      <c r="G5" s="5"/>
     </row>
     <row r="6" spans="2:7" ht="33" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B6" s="7" t="s">
+      <c r="B6" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="C6" s="7" t="s">
+      <c r="C6" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="D6" s="7" t="s">
+      <c r="D6" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="E6" s="7" t="s">
+      <c r="E6" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="F6" s="8" t="s">
+      <c r="F6" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="G6" s="7" t="s">
+      <c r="G6" s="6" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="7" spans="2:7" ht="33" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B7" s="2" t="s">
+      <c r="B7" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="C7" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="D7" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="E7" s="4">
+      <c r="C7" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="E7" s="3">
         <v>0.75</v>
       </c>
-      <c r="F7" s="5">
+      <c r="F7" s="4">
         <f>--(Aufgaben4[[#This Row],[% ABGESCHLOSSEN]]&gt;=1)</f>
         <v>0</v>
       </c>
-      <c r="G7" s="6"/>
+      <c r="G7" s="5"/>
     </row>
     <row r="8" spans="2:7" ht="33" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B8" s="6" t="s">
+      <c r="B8" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="C8" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="D8" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="E8" s="4">
+      <c r="C8" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="E8" s="3">
         <v>0</v>
       </c>
-      <c r="F8" s="5">
+      <c r="F8" s="4">
         <f>--(Aufgaben4[[#This Row],[% ABGESCHLOSSEN]]&gt;=1)</f>
         <v>0</v>
       </c>
-      <c r="G8" s="6"/>
+      <c r="G8" s="5"/>
     </row>
     <row r="9" spans="2:7" ht="33" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B9" s="6" t="s">
+      <c r="B9" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="C9" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="D9" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="E9" s="4">
+      <c r="C9" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D9" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="E9" s="3">
         <v>0</v>
       </c>
-      <c r="F9" s="5">
+      <c r="F9" s="4">
         <f>--(Aufgaben4[[#This Row],[% ABGESCHLOSSEN]]&gt;=1)</f>
         <v>0</v>
       </c>
-      <c r="G9" s="6"/>
+      <c r="G9" s="5"/>
     </row>
     <row r="10" spans="2:7" ht="33" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B10" s="7" t="s">
+      <c r="B10" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="C10" s="7" t="s">
+      <c r="C10" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="D10" s="7" t="s">
+      <c r="D10" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="E10" s="7" t="s">
+      <c r="E10" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="F10" s="8" t="s">
+      <c r="F10" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="G10" s="7" t="s">
+      <c r="G10" s="6" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="11" spans="2:7" ht="33" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B11" s="2" t="s">
+      <c r="B11" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="C11" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="D11" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="E11" s="4">
+      <c r="C11" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D11" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="E11" s="3">
         <v>1</v>
       </c>
-      <c r="F11" s="5">
+      <c r="F11" s="4">
         <f>--(Aufgaben5[[#This Row],[% ABGESCHLOSSEN]]&gt;=1)</f>
         <v>1</v>
       </c>
-      <c r="G11" s="6"/>
+      <c r="G11" s="5"/>
     </row>
     <row r="12" spans="2:7" ht="33" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B12" s="6" t="s">
+      <c r="B12" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="C12" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="D12" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="E12" s="4">
+      <c r="C12" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D12" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="E12" s="3">
         <v>1</v>
       </c>
-      <c r="F12" s="5">
+      <c r="F12" s="4">
         <f>--(Aufgaben5[[#This Row],[% ABGESCHLOSSEN]]&gt;=1)</f>
         <v>1</v>
       </c>
-      <c r="G12" s="6"/>
+      <c r="G12" s="5"/>
     </row>
     <row r="13" spans="2:7" ht="33" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B13" s="6" t="s">
-        <v>0</v>
-      </c>
-      <c r="C13" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="D13" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="E13" s="4">
-        <v>0</v>
-      </c>
-      <c r="F13" s="5">
+      <c r="B13" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="C13" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D13" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="E13" s="3">
+        <v>1</v>
+      </c>
+      <c r="F13" s="4">
         <f>--(Aufgaben5[[#This Row],[% ABGESCHLOSSEN]]&gt;=1)</f>
-        <v>0</v>
-      </c>
-      <c r="G13" s="6"/>
+        <v>1</v>
+      </c>
+      <c r="G13" s="5"/>
+    </row>
+    <row r="14" spans="2:7" ht="33" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B14" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="C14" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D14" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="E14" s="3">
+        <v>1</v>
+      </c>
+      <c r="F14" s="4">
+        <f>--(Aufgaben5[[#This Row],[% ABGESCHLOSSEN]]&gt;=1)</f>
+        <v>1</v>
+      </c>
+      <c r="G14" s="5"/>
+    </row>
+    <row r="15" spans="2:7" ht="33" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B15" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="C15" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D15" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="E15" s="3">
+        <v>1</v>
+      </c>
+      <c r="F15" s="4">
+        <f>--(Aufgaben5[[#This Row],[% ABGESCHLOSSEN]]&gt;=1)</f>
+        <v>1</v>
+      </c>
+      <c r="G15" s="5" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="16" spans="2:7" ht="33" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B16" s="9"/>
+      <c r="C16" s="10"/>
+      <c r="D16" s="10"/>
+      <c r="E16" s="11"/>
+      <c r="F16" s="12"/>
+      <c r="G16" s="9"/>
     </row>
   </sheetData>
   <sheetProtection formatCells="0" formatColumns="0" formatRows="0" insertColumns="0" insertRows="0" deleteColumns="0" deleteRows="0" selectLockedCells="1" sort="0" autoFilter="0"/>
   <mergeCells count="1">
     <mergeCell ref="B1:G1"/>
   </mergeCells>
-  <conditionalFormatting sqref="E3:E5">
+  <conditionalFormatting sqref="E3:E5 E11:E15">
     <cfRule type="dataBar" priority="12">
       <dataBar>
         <cfvo type="num" val="0"/>
@@ -1673,22 +1756,8 @@
       </extLst>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E11:E13">
-    <cfRule type="dataBar" priority="1">
-      <dataBar>
-        <cfvo type="num" val="0"/>
-        <cfvo type="num" val="1"/>
-        <color theme="5"/>
-      </dataBar>
-      <extLst>
-        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
-          <x14:id>{0E93B563-EDCC-FF4C-BB00-6DDFDC2727B7}</x14:id>
-        </ext>
-      </extLst>
-    </cfRule>
-  </conditionalFormatting>
   <dataValidations xWindow="542" yWindow="341" count="1">
-    <dataValidation type="list" errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Wählen Sie einen Wert aus der Dropdownliste aus oder geben Sie eine der folgenden Optionen ein: 0 %, 25 %, 50 %, 75 % oder 100 %" sqref="E3:E5 E7:E9 E11:E13" xr:uid="{00000000-0002-0000-0000-000000000000}">
+    <dataValidation type="list" errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Wählen Sie einen Wert aus der Dropdownliste aus oder geben Sie eine der folgenden Optionen ein: 0 %, 25 %, 50 %, 75 % oder 100 %" sqref="E3:E5 E7:E9 E11:E15" xr:uid="{00000000-0002-0000-0000-000000000000}">
       <formula1>"0%,25%,50%,75%,100%"</formula1>
     </dataValidation>
   </dataValidations>
@@ -1722,7 +1791,24 @@
               <x14:axisColor rgb="FF000000"/>
             </x14:dataBar>
           </x14:cfRule>
-          <xm:sqref>E3:E5</xm:sqref>
+          <xm:sqref>E3:E5 E11:E15</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="dataBar" id="{44967FC8-DD27-4844-A69F-821551C0039D}">
+            <x14:dataBar minLength="0" maxLength="100" border="1" gradient="0" negativeBarBorderColorSameAsPositive="0">
+              <x14:cfvo type="num">
+                <xm:f>0</xm:f>
+              </x14:cfvo>
+              <x14:cfvo type="num">
+                <xm:f>1</xm:f>
+              </x14:cfvo>
+              <x14:borderColor theme="5"/>
+              <x14:negativeFillColor rgb="FFFF0000"/>
+              <x14:negativeBorderColor rgb="FFFF0000"/>
+              <x14:axisColor rgb="FF000000"/>
+            </x14:dataBar>
+          </x14:cfRule>
+          <xm:sqref>E7:E9</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
           <x14:cfRule type="iconSet" priority="47" id="{04B8B5C2-C7B5-4FE5-B018-764654046486}">
@@ -1744,23 +1830,6 @@
           <xm:sqref>F3:F5</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="dataBar" id="{44967FC8-DD27-4844-A69F-821551C0039D}">
-            <x14:dataBar minLength="0" maxLength="100" border="1" gradient="0" negativeBarBorderColorSameAsPositive="0">
-              <x14:cfvo type="num">
-                <xm:f>0</xm:f>
-              </x14:cfvo>
-              <x14:cfvo type="num">
-                <xm:f>1</xm:f>
-              </x14:cfvo>
-              <x14:borderColor theme="5"/>
-              <x14:negativeFillColor rgb="FFFF0000"/>
-              <x14:negativeBorderColor rgb="FFFF0000"/>
-              <x14:axisColor rgb="FF000000"/>
-            </x14:dataBar>
-          </x14:cfRule>
-          <xm:sqref>E7:E9</xm:sqref>
-        </x14:conditionalFormatting>
-        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
           <x14:cfRule type="iconSet" priority="4" id="{DEA2C51E-1846-A244-99D3-35CA1F3A339D}">
             <x14:iconSet custom="1">
               <x14:cfvo type="percent">
@@ -1780,24 +1849,7 @@
           <xm:sqref>F7:F9</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="dataBar" id="{0E93B563-EDCC-FF4C-BB00-6DDFDC2727B7}">
-            <x14:dataBar minLength="0" maxLength="100" border="1" gradient="0" negativeBarBorderColorSameAsPositive="0">
-              <x14:cfvo type="num">
-                <xm:f>0</xm:f>
-              </x14:cfvo>
-              <x14:cfvo type="num">
-                <xm:f>1</xm:f>
-              </x14:cfvo>
-              <x14:borderColor theme="5"/>
-              <x14:negativeFillColor rgb="FFFF0000"/>
-              <x14:negativeBorderColor rgb="FFFF0000"/>
-              <x14:axisColor rgb="FF000000"/>
-            </x14:dataBar>
-          </x14:cfRule>
-          <xm:sqref>E11:E13</xm:sqref>
-        </x14:conditionalFormatting>
-        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="iconSet" priority="2" id="{885FA9AE-EDD0-254E-A199-B5BF46D76240}">
+          <x14:cfRule type="iconSet" priority="59" id="{885FA9AE-EDD0-254E-A199-B5BF46D76240}">
             <x14:iconSet custom="1">
               <x14:cfvo type="percent">
                 <xm:f>0</xm:f>
@@ -1813,7 +1865,7 @@
               <x14:cfIcon iconSet="4TrafficLights" iconId="0"/>
             </x14:iconSet>
           </x14:cfRule>
-          <xm:sqref>F11:F13</xm:sqref>
+          <xm:sqref>F11:F15</xm:sqref>
         </x14:conditionalFormatting>
       </x14:conditionalFormattings>
     </ext>

</xml_diff>